<commit_message>
move files to project folder
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Afgangsprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B398A01C-B39C-4D45-ADBE-E4FDC18738E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E675FBD-271C-46D8-86FD-30081F44E818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36170" yWindow="790" windowWidth="11220" windowHeight="12850" xr2:uid="{BA66CC56-D44A-4480-9CC8-12B39CE1E54D}"/>
+    <workbookView xWindow="-31600" yWindow="140" windowWidth="28800" windowHeight="15440" xr2:uid="{BA66CC56-D44A-4480-9CC8-12B39CE1E54D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Todo:</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Skriv ind at vi benytter threshold på 0,25 i TF</t>
+  </si>
+  <si>
+    <t>State space</t>
+  </si>
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>Skriv kode referencer</t>
   </si>
 </sst>
 </file>
@@ -448,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF1BC5C-AE1F-4724-8234-D08576F0A133}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -529,6 +538,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
@@ -562,6 +576,16 @@
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>